<commit_message>
unique() fix and template updates
</commit_message>
<xml_diff>
--- a/test_files/Specimen_Example.xlsx
+++ b/test_files/Specimen_Example.xlsx
@@ -10,7 +10,7 @@
   <sheets>
     <sheet name="test_specimen_simplified" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="R1C1" iterate="false" iterateDelta="0.001"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelR1C1"/>
@@ -20,7 +20,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="87">
+  <si>
+    <t xml:space="preserve">AdditionalMetaData</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RawData</t>
+  </si>
   <si>
     <t xml:space="preserve">Specimen</t>
   </si>
@@ -46,7 +52,7 @@
     <t xml:space="preserve">CollectionSite</t>
   </si>
   <si>
-    <t xml:space="preserve">AdditionalMetaData</t>
+    <t xml:space="preserve">SubjectIdCol</t>
   </si>
   <si>
     <t xml:space="preserve">BarcodeSequence</t>
@@ -55,7 +61,7 @@
     <t xml:space="preserve">LinkerPrimerSequence</t>
   </si>
   <si>
-    <t xml:space="preserve">SpecimenID</t>
+    <t xml:space="preserve">RawDataID</t>
   </si>
   <si>
     <t xml:space="preserve">SpecimenNotes</t>
@@ -100,16 +106,13 @@
     <t xml:space="preserve">CollectionSiteTechnician</t>
   </si>
   <si>
-    <t xml:space="preserve">SubjectIdCol</t>
-  </si>
-  <si>
     <t xml:space="preserve">Your_Column_Here</t>
   </si>
   <si>
+    <t xml:space="preserve">Optional</t>
+  </si>
+  <si>
     <t xml:space="preserve">Required</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Optional</t>
   </si>
   <si>
     <t xml:space="preserve">Text</t>
@@ -293,6 +296,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -314,6 +318,7 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -390,23 +395,22 @@
   </sheetPr>
   <dimension ref="A1:S21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R24" activeCellId="0" sqref="R24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="81.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="21.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="7" style="0" width="18.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="10" style="0" width="17.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="22.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="14" style="0" width="17.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="21.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="18.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="18.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="81.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="21.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="8" style="0" width="18.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="11" style="0" width="17.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="22.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="15" style="0" width="17.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="21.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="43.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="18.24"/>
   </cols>
@@ -416,131 +420,131 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="R1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="S1" s="0" t="s">
         <v>0</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="L1" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="M1" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="N1" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="O1" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="P1" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q1" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="R1" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="S1" s="0" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="R2" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="S2" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>29</v>
@@ -561,19 +565,19 @@
         <v>29</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="O3" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="P3" s="0" t="s">
         <v>29</v>
@@ -590,75 +594,75 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>31</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N4" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="O4" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="P4" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Q4" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="R4" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="S4" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>33</v>
@@ -667,48 +671,48 @@
         <v>34</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="N5" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="O5" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="P5" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="Q5" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="R5" s="0" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="S5" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>35</v>
+      <c r="A6" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>36</v>
@@ -719,11 +723,11 @@
       <c r="D6" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="1" t="n">
+      <c r="E6" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="1" t="n">
         <v>44197</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>39</v>
       </c>
       <c r="G6" s="0" t="s">
         <v>40</v>
@@ -743,10 +747,10 @@
       <c r="L6" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="M6" s="2" t="s">
+      <c r="M6" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="N6" s="0" t="s">
+      <c r="N6" s="2" t="s">
         <v>47</v>
       </c>
       <c r="O6" s="0" t="s">
@@ -758,31 +762,31 @@
       <c r="Q6" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="R6" s="0" t="n">
-        <v>1</v>
+      <c r="R6" s="0" t="s">
+        <v>51</v>
       </c>
       <c r="S6" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>52</v>
+      <c r="A7" s="0" t="n">
+        <v>2</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="E7" s="1" t="n">
+      <c r="E7" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" s="1" t="n">
         <v>44198</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>39</v>
       </c>
       <c r="G7" s="0" t="s">
         <v>40</v>
@@ -802,10 +806,10 @@
       <c r="L7" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="M7" s="2" t="s">
+      <c r="M7" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="N7" s="0" t="s">
+      <c r="N7" s="2" t="s">
         <v>47</v>
       </c>
       <c r="O7" s="0" t="s">
@@ -817,31 +821,31 @@
       <c r="Q7" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="R7" s="0" t="n">
+      <c r="R7" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="S7" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="S7" s="0" t="s">
+      <c r="B8" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="0" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="E8" s="1" t="n">
+      <c r="F8" s="1" t="n">
         <v>44199</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>39</v>
       </c>
       <c r="G8" s="0" t="s">
         <v>40</v>
@@ -861,10 +865,10 @@
       <c r="L8" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="M8" s="2" t="s">
+      <c r="M8" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="N8" s="0" t="s">
+      <c r="N8" s="2" t="s">
         <v>47</v>
       </c>
       <c r="O8" s="0" t="s">
@@ -876,31 +880,31 @@
       <c r="Q8" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="R8" s="0" t="n">
-        <v>2</v>
+      <c r="R8" s="0" t="s">
+        <v>51</v>
       </c>
       <c r="S8" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>59</v>
+      <c r="A9" s="0" t="n">
+        <v>3</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="E9" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="F9" s="1" t="n">
         <v>44200</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>39</v>
       </c>
       <c r="G9" s="0" t="s">
         <v>40</v>
@@ -920,10 +924,10 @@
       <c r="L9" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="M9" s="2" t="s">
+      <c r="M9" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="N9" s="0" t="s">
+      <c r="N9" s="2" t="s">
         <v>47</v>
       </c>
       <c r="O9" s="0" t="s">
@@ -935,31 +939,31 @@
       <c r="Q9" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="R9" s="0" t="n">
-        <v>3</v>
+      <c r="R9" s="0" t="s">
+        <v>51</v>
       </c>
       <c r="S9" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>61</v>
+      <c r="A10" s="0" t="n">
+        <v>4</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>62</v>
+        <v>37</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="E10" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" s="1" t="n">
         <v>44201</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>39</v>
       </c>
       <c r="G10" s="0" t="s">
         <v>40</v>
@@ -979,10 +983,10 @@
       <c r="L10" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="M10" s="2" t="s">
+      <c r="M10" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="N10" s="0" t="s">
+      <c r="N10" s="2" t="s">
         <v>47</v>
       </c>
       <c r="O10" s="0" t="s">
@@ -994,31 +998,31 @@
       <c r="Q10" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="R10" s="0" t="n">
-        <v>4</v>
+      <c r="R10" s="0" t="s">
+        <v>51</v>
       </c>
       <c r="S10" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11" s="0" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="E11" s="1" t="n">
+      <c r="F11" s="1" t="n">
         <v>44202</v>
-      </c>
-      <c r="F11" s="0" t="s">
-        <v>39</v>
       </c>
       <c r="G11" s="0" t="s">
         <v>40</v>
@@ -1038,10 +1042,10 @@
       <c r="L11" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="M11" s="2" t="s">
+      <c r="M11" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="N11" s="0" t="s">
+      <c r="N11" s="2" t="s">
         <v>47</v>
       </c>
       <c r="O11" s="0" t="s">
@@ -1053,31 +1057,31 @@
       <c r="Q11" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="R11" s="0" t="n">
-        <v>5</v>
+      <c r="R11" s="0" t="s">
+        <v>51</v>
       </c>
       <c r="S11" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>65</v>
+      <c r="A12" s="0" t="n">
+        <v>6</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>66</v>
+        <v>37</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="E12" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" s="1" t="n">
         <v>44203</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>39</v>
       </c>
       <c r="G12" s="0" t="s">
         <v>40</v>
@@ -1097,10 +1101,10 @@
       <c r="L12" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="M12" s="2" t="s">
+      <c r="M12" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="N12" s="0" t="s">
+      <c r="N12" s="2" t="s">
         <v>47</v>
       </c>
       <c r="O12" s="0" t="s">
@@ -1112,31 +1116,31 @@
       <c r="Q12" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="R12" s="0" t="n">
-        <v>6</v>
+      <c r="R12" s="0" t="s">
+        <v>51</v>
       </c>
       <c r="S12" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>67</v>
+      <c r="A13" s="0" t="n">
+        <v>7</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>36</v>
+        <v>68</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="E13" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" s="1" t="n">
         <v>44204</v>
-      </c>
-      <c r="F13" s="0" t="s">
-        <v>39</v>
       </c>
       <c r="G13" s="0" t="s">
         <v>40</v>
@@ -1156,10 +1160,10 @@
       <c r="L13" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="M13" s="2" t="s">
+      <c r="M13" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="N13" s="0" t="s">
+      <c r="N13" s="2" t="s">
         <v>47</v>
       </c>
       <c r="O13" s="0" t="s">
@@ -1171,31 +1175,31 @@
       <c r="Q13" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="R13" s="0" t="n">
-        <v>7</v>
+      <c r="R13" s="0" t="s">
+        <v>51</v>
       </c>
       <c r="S13" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="E14" s="0" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="E14" s="1" t="n">
+      <c r="F14" s="1" t="n">
         <v>44205</v>
-      </c>
-      <c r="F14" s="0" t="s">
-        <v>39</v>
       </c>
       <c r="G14" s="0" t="s">
         <v>40</v>
@@ -1215,10 +1219,10 @@
       <c r="L14" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="M14" s="2" t="s">
+      <c r="M14" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="N14" s="0" t="s">
+      <c r="N14" s="2" t="s">
         <v>47</v>
       </c>
       <c r="O14" s="0" t="s">
@@ -1230,31 +1234,31 @@
       <c r="Q14" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="R14" s="0" t="n">
-        <v>8</v>
+      <c r="R14" s="0" t="s">
+        <v>51</v>
       </c>
       <c r="S14" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>71</v>
+      <c r="A15" s="0" t="n">
+        <v>9</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>72</v>
+        <v>37</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="E15" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="F15" s="1" t="n">
         <v>44206</v>
-      </c>
-      <c r="F15" s="0" t="s">
-        <v>39</v>
       </c>
       <c r="G15" s="0" t="s">
         <v>40</v>
@@ -1274,10 +1278,10 @@
       <c r="L15" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="M15" s="2" t="s">
+      <c r="M15" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="N15" s="0" t="s">
+      <c r="N15" s="2" t="s">
         <v>47</v>
       </c>
       <c r="O15" s="0" t="s">
@@ -1289,31 +1293,31 @@
       <c r="Q15" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="R15" s="0" t="n">
-        <v>9</v>
+      <c r="R15" s="0" t="s">
+        <v>51</v>
       </c>
       <c r="S15" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>73</v>
+      <c r="A16" s="0" t="n">
+        <v>10</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>36</v>
+        <v>74</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="E16" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="F16" s="1" t="n">
         <v>44207</v>
-      </c>
-      <c r="F16" s="0" t="s">
-        <v>39</v>
       </c>
       <c r="G16" s="0" t="s">
         <v>40</v>
@@ -1333,10 +1337,10 @@
       <c r="L16" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="M16" s="2" t="s">
+      <c r="M16" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="N16" s="0" t="s">
+      <c r="N16" s="2" t="s">
         <v>47</v>
       </c>
       <c r="O16" s="0" t="s">
@@ -1348,31 +1352,31 @@
       <c r="Q16" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="R16" s="0" t="n">
-        <v>10</v>
+      <c r="R16" s="0" t="s">
+        <v>51</v>
       </c>
       <c r="S16" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="E17" s="0" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="E17" s="1" t="n">
+      <c r="F17" s="1" t="n">
         <v>44208</v>
-      </c>
-      <c r="F17" s="0" t="s">
-        <v>39</v>
       </c>
       <c r="G17" s="0" t="s">
         <v>40</v>
@@ -1392,10 +1396,10 @@
       <c r="L17" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="M17" s="2" t="s">
+      <c r="M17" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="N17" s="0" t="s">
+      <c r="N17" s="2" t="s">
         <v>47</v>
       </c>
       <c r="O17" s="0" t="s">
@@ -1407,31 +1411,31 @@
       <c r="Q17" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="R17" s="0" t="n">
-        <v>11</v>
+      <c r="R17" s="0" t="s">
+        <v>51</v>
       </c>
       <c r="S17" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>77</v>
+      <c r="A18" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>36</v>
+        <v>78</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>78</v>
+        <v>37</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="E18" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="F18" s="1" t="n">
         <v>44209</v>
-      </c>
-      <c r="F18" s="0" t="s">
-        <v>39</v>
       </c>
       <c r="G18" s="0" t="s">
         <v>40</v>
@@ -1451,10 +1455,10 @@
       <c r="L18" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="M18" s="2" t="s">
+      <c r="M18" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="N18" s="0" t="s">
+      <c r="N18" s="2" t="s">
         <v>47</v>
       </c>
       <c r="O18" s="0" t="s">
@@ -1466,31 +1470,31 @@
       <c r="Q18" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="R18" s="0" t="n">
-        <v>1</v>
+      <c r="R18" s="0" t="s">
+        <v>51</v>
       </c>
       <c r="S18" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>79</v>
+      <c r="A19" s="0" t="n">
+        <v>2</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>36</v>
+        <v>80</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>80</v>
+        <v>37</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="E19" s="1" t="n">
+      <c r="E19" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="F19" s="1" t="n">
         <v>44210</v>
-      </c>
-      <c r="F19" s="0" t="s">
-        <v>39</v>
       </c>
       <c r="G19" s="0" t="s">
         <v>40</v>
@@ -1510,10 +1514,10 @@
       <c r="L19" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="M19" s="2" t="s">
+      <c r="M19" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="N19" s="0" t="s">
+      <c r="N19" s="2" t="s">
         <v>47</v>
       </c>
       <c r="O19" s="0" t="s">
@@ -1525,31 +1529,31 @@
       <c r="Q19" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="R19" s="0" t="n">
-        <v>2</v>
+      <c r="R19" s="0" t="s">
+        <v>51</v>
       </c>
       <c r="S19" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="E20" s="0" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="E20" s="1" t="n">
+      <c r="F20" s="1" t="n">
         <v>44211</v>
-      </c>
-      <c r="F20" s="0" t="s">
-        <v>39</v>
       </c>
       <c r="G20" s="0" t="s">
         <v>40</v>
@@ -1569,10 +1573,10 @@
       <c r="L20" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="M20" s="2" t="s">
+      <c r="M20" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="N20" s="0" t="s">
+      <c r="N20" s="2" t="s">
         <v>47</v>
       </c>
       <c r="O20" s="0" t="s">
@@ -1584,31 +1588,31 @@
       <c r="Q20" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="R20" s="0" t="n">
-        <v>3</v>
+      <c r="R20" s="0" t="s">
+        <v>51</v>
       </c>
       <c r="S20" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>84</v>
+      <c r="A21" s="0" t="n">
+        <v>7</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>36</v>
+        <v>85</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>85</v>
+        <v>37</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="E21" s="1" t="n">
+        <v>86</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="F21" s="1" t="n">
         <v>44212</v>
-      </c>
-      <c r="F21" s="0" t="s">
-        <v>39</v>
       </c>
       <c r="G21" s="0" t="s">
         <v>40</v>
@@ -1628,10 +1632,10 @@
       <c r="L21" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="M21" s="2" t="s">
+      <c r="M21" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="N21" s="0" t="s">
+      <c r="N21" s="2" t="s">
         <v>47</v>
       </c>
       <c r="O21" s="0" t="s">
@@ -1643,31 +1647,31 @@
       <c r="Q21" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="R21" s="0" t="n">
-        <v>7</v>
+      <c r="R21" s="0" t="s">
+        <v>51</v>
       </c>
       <c r="S21" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M6" r:id="rId1" display="david.wallach@mssm.edu"/>
-    <hyperlink ref="M7" r:id="rId2" display="david.wallach@mssm.edu"/>
-    <hyperlink ref="M8" r:id="rId3" display="david.wallach@mssm.edu"/>
-    <hyperlink ref="M9" r:id="rId4" display="david.wallach@mssm.edu"/>
-    <hyperlink ref="M10" r:id="rId5" display="david.wallach@mssm.edu"/>
-    <hyperlink ref="M11" r:id="rId6" display="david.wallach@mssm.edu"/>
-    <hyperlink ref="M12" r:id="rId7" display="david.wallach@mssm.edu"/>
-    <hyperlink ref="M13" r:id="rId8" display="david.wallach@mssm.edu"/>
-    <hyperlink ref="M14" r:id="rId9" display="david.wallach@mssm.edu"/>
-    <hyperlink ref="M15" r:id="rId10" display="david.wallach@mssm.edu"/>
-    <hyperlink ref="M16" r:id="rId11" display="david.wallach@mssm.edu"/>
-    <hyperlink ref="M17" r:id="rId12" display="david.wallach@mssm.edu"/>
-    <hyperlink ref="M18" r:id="rId13" display="david.wallach@mssm.edu"/>
-    <hyperlink ref="M19" r:id="rId14" display="david.wallach@mssm.edu"/>
-    <hyperlink ref="M20" r:id="rId15" display="david.wallach@mssm.edu"/>
-    <hyperlink ref="M21" r:id="rId16" display="david.wallach@mssm.edu"/>
+    <hyperlink ref="N6" r:id="rId1" display="david.wallach@mssm.edu"/>
+    <hyperlink ref="N7" r:id="rId2" display="david.wallach@mssm.edu"/>
+    <hyperlink ref="N8" r:id="rId3" display="david.wallach@mssm.edu"/>
+    <hyperlink ref="N9" r:id="rId4" display="david.wallach@mssm.edu"/>
+    <hyperlink ref="N10" r:id="rId5" display="david.wallach@mssm.edu"/>
+    <hyperlink ref="N11" r:id="rId6" display="david.wallach@mssm.edu"/>
+    <hyperlink ref="N12" r:id="rId7" display="david.wallach@mssm.edu"/>
+    <hyperlink ref="N13" r:id="rId8" display="david.wallach@mssm.edu"/>
+    <hyperlink ref="N14" r:id="rId9" display="david.wallach@mssm.edu"/>
+    <hyperlink ref="N15" r:id="rId10" display="david.wallach@mssm.edu"/>
+    <hyperlink ref="N16" r:id="rId11" display="david.wallach@mssm.edu"/>
+    <hyperlink ref="N17" r:id="rId12" display="david.wallach@mssm.edu"/>
+    <hyperlink ref="N18" r:id="rId13" display="david.wallach@mssm.edu"/>
+    <hyperlink ref="N19" r:id="rId14" display="david.wallach@mssm.edu"/>
+    <hyperlink ref="N20" r:id="rId15" display="david.wallach@mssm.edu"/>
+    <hyperlink ref="N21" r:id="rId16" display="david.wallach@mssm.edu"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>